<commit_message>
Agregando punto 3.1 al plan de gestion de configuracion
</commit_message>
<xml_diff>
--- a/DESARROLLO/SAV/GESTION/SAV-CP.xlsx
+++ b/DESARROLLO/SAV/GESTION/SAV-CP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="2592" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Fase de inicio</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Estimar historias de usuario</t>
+  </si>
+  <si>
+    <t>Aprobar actas del proyecto</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,8 @@
   <dimension ref="A1:BX173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A27" sqref="A27"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG20" sqref="AG20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,12 +765,10 @@
         <v>43727</v>
       </c>
       <c r="C3" s="12">
-        <v>43740</v>
+        <v>43728</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="Q3" s="11"/>
       <c r="BK3" s="3"/>
       <c r="BL3" s="3"/>
       <c r="BM3" s="3"/>
@@ -831,6 +832,7 @@
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
       <c r="BK6" s="3"/>
       <c r="BL6" s="3"/>
       <c r="BM6" s="3"/>
@@ -904,6 +906,16 @@
       <c r="BR9" s="3"/>
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="12">
+        <v>43740</v>
+      </c>
+      <c r="C10" s="12">
+        <v>43740</v>
+      </c>
+      <c r="Q10" s="11"/>
       <c r="BK10" s="3"/>
       <c r="BL10" s="3"/>
       <c r="BM10" s="3"/>
@@ -914,12 +926,6 @@
       <c r="BR10" s="3"/>
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
       <c r="BK11" s="3"/>
       <c r="BL11" s="3"/>
       <c r="BM11" s="3"/>
@@ -930,19 +936,12 @@
       <c r="BR11" s="3"/>
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="12">
-        <v>43741</v>
-      </c>
-      <c r="C12" s="12">
-        <v>43743</v>
-      </c>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="V12" s="3"/>
+      <c r="A12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
       <c r="BM12" s="3"/>
@@ -954,19 +953,18 @@
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="12">
-        <v>43744</v>
+        <v>43741</v>
       </c>
       <c r="C13" s="12">
-        <v>43746</v>
-      </c>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="Z13" s="3"/>
-      <c r="AO13" s="3"/>
+        <v>43743</v>
+      </c>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="V13" s="3"/>
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
       <c r="BM13" s="3"/>
@@ -978,17 +976,19 @@
     </row>
     <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B14" s="12">
-        <v>43747</v>
+        <v>43744</v>
       </c>
       <c r="C14" s="12">
-        <v>43748</v>
-      </c>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
+        <v>43746</v>
+      </c>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
       <c r="Z14" s="3"/>
+      <c r="AO14" s="3"/>
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
       <c r="BM14" s="3"/>
@@ -1000,16 +1000,17 @@
     </row>
     <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B15" s="12">
-        <v>43749</v>
+        <v>43747</v>
       </c>
       <c r="C15" s="12">
-        <v>43750</v>
-      </c>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
+        <v>43748</v>
+      </c>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="3"/>
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
       <c r="BM15" s="3"/>
@@ -1021,14 +1022,15 @@
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="12">
-        <v>43750</v>
+        <v>43749</v>
       </c>
       <c r="C16" s="12">
         <v>43750</v>
       </c>
+      <c r="Z16" s="11"/>
       <c r="AA16" s="11"/>
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
@@ -1041,21 +1043,15 @@
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B17" s="12">
-        <v>43758</v>
+        <v>43750</v>
       </c>
       <c r="C17" s="12">
-        <v>43766</v>
-      </c>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
-      <c r="AI17" s="11"/>
-      <c r="AJ17" s="11"/>
+        <v>43750</v>
+      </c>
+      <c r="AA17" s="11"/>
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
       <c r="BM17" s="3"/>
@@ -1067,18 +1063,21 @@
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B18" s="12">
-        <v>43761</v>
+        <v>43758</v>
       </c>
       <c r="C18" s="12">
-        <v>43768</v>
-      </c>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AK18" s="11"/>
-      <c r="AL18" s="11"/>
+        <v>43766</v>
+      </c>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
       <c r="BK18" s="3"/>
       <c r="BL18" s="3"/>
       <c r="BM18" s="3"/>
@@ -1089,16 +1088,19 @@
       <c r="BR18" s="3"/>
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
+      <c r="A19" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B19" s="12">
-        <v>43770</v>
+        <v>43761</v>
       </c>
       <c r="C19" s="12">
-        <v>43770</v>
-      </c>
-      <c r="AM19" s="11"/>
+        <v>43768</v>
+      </c>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11"/>
       <c r="BK19" s="3"/>
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
@@ -1109,6 +1111,16 @@
       <c r="BR19" s="3"/>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="12">
+        <v>43770</v>
+      </c>
+      <c r="C20" s="12">
+        <v>43770</v>
+      </c>
+      <c r="AM20" s="11"/>
       <c r="BK20" s="3"/>
       <c r="BL20" s="3"/>
       <c r="BM20" s="3"/>
@@ -1119,9 +1131,6 @@
       <c r="BR20" s="3"/>
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="BK21" s="3"/>
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
@@ -1132,22 +1141,9 @@
       <c r="BR21" s="3"/>
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="12">
-        <v>43771</v>
-      </c>
-      <c r="C22" s="12">
-        <v>43777</v>
-      </c>
-      <c r="AN22" s="11"/>
-      <c r="AO22" s="11"/>
-      <c r="AP22" s="11"/>
-      <c r="AQ22" s="11"/>
-      <c r="AR22" s="11"/>
-      <c r="AS22" s="11"/>
-      <c r="AT22" s="11"/>
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="BK22" s="3"/>
       <c r="BL22" s="3"/>
       <c r="BM22" s="3"/>
@@ -1158,22 +1154,22 @@
       <c r="BR22" s="3"/>
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>28</v>
+      <c r="A23" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B23" s="12">
-        <v>43778</v>
+        <v>43771</v>
       </c>
       <c r="C23" s="12">
-        <v>43784</v>
-      </c>
-      <c r="AU23" s="11"/>
-      <c r="AV23" s="11"/>
-      <c r="AW23" s="11"/>
-      <c r="AX23" s="11"/>
-      <c r="AY23" s="11"/>
-      <c r="AZ23" s="11"/>
-      <c r="BA23" s="11"/>
+        <v>43777</v>
+      </c>
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11"/>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="11"/>
+      <c r="AS23" s="11"/>
+      <c r="AT23" s="11"/>
       <c r="BK23" s="3"/>
       <c r="BL23" s="3"/>
       <c r="BM23" s="3"/>
@@ -1184,6 +1180,22 @@
       <c r="BR23" s="3"/>
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="12">
+        <v>43778</v>
+      </c>
+      <c r="C24" s="12">
+        <v>43784</v>
+      </c>
+      <c r="AU24" s="11"/>
+      <c r="AV24" s="11"/>
+      <c r="AW24" s="11"/>
+      <c r="AX24" s="11"/>
+      <c r="AY24" s="11"/>
+      <c r="AZ24" s="11"/>
+      <c r="BA24" s="11"/>
       <c r="BK24" s="3"/>
       <c r="BL24" s="3"/>
       <c r="BM24" s="3"/>
@@ -1194,9 +1206,6 @@
       <c r="BR24" s="3"/>
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="BK25" s="3"/>
       <c r="BL25" s="3"/>
       <c r="BM25" s="3"/>
@@ -1207,17 +1216,9 @@
       <c r="BR25" s="3"/>
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="12">
-        <v>43785</v>
-      </c>
-      <c r="C26" s="12">
-        <v>43786</v>
-      </c>
-      <c r="BB26" s="11"/>
-      <c r="BC26" s="11"/>
+      <c r="A26" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="BK26" s="3"/>
       <c r="BL26" s="3"/>
       <c r="BM26" s="3"/>
@@ -1229,16 +1230,15 @@
     </row>
     <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" s="12">
-        <v>43786</v>
+        <v>43785</v>
       </c>
       <c r="C27" s="12">
         <v>43786</v>
       </c>
-      <c r="AW27" s="3"/>
-      <c r="AX27" s="3"/>
+      <c r="BB27" s="11"/>
       <c r="BC27" s="11"/>
       <c r="BK27" s="3"/>
       <c r="BL27" s="3"/>
@@ -1251,18 +1251,17 @@
     </row>
     <row r="28" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" s="12">
-        <v>43787</v>
+        <v>43786</v>
       </c>
       <c r="C28" s="12">
-        <v>43788</v>
+        <v>43786</v>
       </c>
       <c r="AW28" s="3"/>
       <c r="AX28" s="3"/>
-      <c r="BD28" s="11"/>
-      <c r="BE28" s="11"/>
+      <c r="BC28" s="11"/>
       <c r="BK28" s="3"/>
       <c r="BL28" s="3"/>
       <c r="BM28" s="3"/>
@@ -1273,18 +1272,19 @@
       <c r="BR28" s="3"/>
     </row>
     <row r="29" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>37</v>
+      <c r="A29" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B29" s="12">
-        <v>43789</v>
+        <v>43787</v>
       </c>
       <c r="C29" s="12">
-        <v>43789</v>
+        <v>43788</v>
       </c>
       <c r="AW29" s="3"/>
       <c r="AX29" s="3"/>
-      <c r="BF29" s="11"/>
+      <c r="BD29" s="11"/>
+      <c r="BE29" s="11"/>
       <c r="BK29" s="3"/>
       <c r="BL29" s="3"/>
       <c r="BM29" s="3"/>
@@ -1295,8 +1295,8 @@
       <c r="BR29" s="3"/>
     </row>
     <row r="30" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>36</v>
+      <c r="A30" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="B30" s="12">
         <v>43789</v>
@@ -1317,6 +1317,18 @@
       <c r="BR30" s="3"/>
     </row>
     <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="12">
+        <v>43789</v>
+      </c>
+      <c r="C31" s="12">
+        <v>43789</v>
+      </c>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="3"/>
+      <c r="BF31" s="11"/>
       <c r="BK31" s="3"/>
       <c r="BL31" s="3"/>
       <c r="BM31" s="3"/>
@@ -1327,9 +1339,6 @@
       <c r="BR31" s="3"/>
     </row>
     <row r="32" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="BK32" s="3"/>
       <c r="BL32" s="3"/>
       <c r="BM32" s="3"/>
@@ -1340,17 +1349,9 @@
       <c r="BR32" s="3"/>
     </row>
     <row r="33" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="12">
-        <v>43790</v>
-      </c>
-      <c r="C33" s="12">
-        <v>43791</v>
-      </c>
-      <c r="BG33" s="11"/>
-      <c r="BH33" s="11"/>
+      <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="BK33" s="3"/>
       <c r="BL33" s="3"/>
       <c r="BM33" s="3"/>
@@ -1361,16 +1362,17 @@
       <c r="BR33" s="3"/>
     </row>
     <row r="34" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>39</v>
+      <c r="A34" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B34" s="12">
-        <v>43792</v>
+        <v>43790</v>
       </c>
       <c r="C34" s="12">
-        <v>43792</v>
-      </c>
-      <c r="BI34" s="11"/>
+        <v>43791</v>
+      </c>
+      <c r="BG34" s="11"/>
+      <c r="BH34" s="11"/>
       <c r="BK34" s="3"/>
       <c r="BL34" s="3"/>
       <c r="BM34" s="3"/>
@@ -1382,15 +1384,15 @@
     </row>
     <row r="35" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35" s="12">
-        <v>43793</v>
+        <v>43792</v>
       </c>
       <c r="C35" s="12">
-        <v>43793</v>
-      </c>
-      <c r="BJ35" s="11"/>
+        <v>43792</v>
+      </c>
+      <c r="BI35" s="11"/>
       <c r="BK35" s="3"/>
       <c r="BL35" s="3"/>
       <c r="BM35" s="3"/>
@@ -1401,8 +1403,8 @@
       <c r="BR35" s="3"/>
     </row>
     <row r="36" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>42</v>
+      <c r="A36" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="B36" s="12">
         <v>43793</v>
@@ -1421,7 +1423,16 @@
       <c r="BR36" s="3"/>
     </row>
     <row r="37" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
+      <c r="A37" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="12">
+        <v>43793</v>
+      </c>
+      <c r="C37" s="12">
+        <v>43793</v>
+      </c>
+      <c r="BJ37" s="11"/>
     </row>
     <row r="38" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>

</xml_diff>

<commit_message>
Modificacion de responsable cronograma
</commit_message>
<xml_diff>
--- a/DESARROLLO/SAV/GESTION/SAV-CP.xlsx
+++ b/DESARROLLO/SAV/GESTION/SAV-CP.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
   <si>
     <t xml:space="preserve">RESPONSABLE</t>
   </si>
@@ -83,6 +83,9 @@
     <t xml:space="preserve">Estimar historias de usuario (Documento de presupuestos) *</t>
   </si>
   <si>
+    <t xml:space="preserve">Giordano Barbieri Lizama</t>
+  </si>
+  <si>
     <t xml:space="preserve">Definir las iteraciones e historias de usuario por iteración</t>
   </si>
   <si>
@@ -143,7 +146,7 @@
     <t xml:space="preserve">Giordano Barbieri</t>
   </si>
   <si>
-    <t xml:space="preserve">Jhon Alex</t>
+    <t xml:space="preserve">Jhon Alex Quispe</t>
   </si>
   <si>
     <t xml:space="preserve">Fase de lanzamiento</t>
@@ -492,10 +495,10 @@
   </sheetPr>
   <dimension ref="A1:DU185"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topRight" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1258,12 +1261,12 @@
       <c r="BT16" s="15"/>
       <c r="BU16" s="15"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C17" s="12" t="n">
         <v>43747</v>
@@ -1288,7 +1291,7 @@
     <row r="18" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C18" s="12" t="n">
         <v>43794</v>
@@ -1308,9 +1311,9 @@
       <c r="BR18" s="1"/>
       <c r="BS18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>8</v>
@@ -1351,7 +1354,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>16</v>
@@ -1394,10 +1397,10 @@
     </row>
     <row r="23" customFormat="false" ht="40.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" s="12" t="n">
         <v>43758</v>
@@ -1424,7 +1427,7 @@
     <row r="24" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
       <c r="B24" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="12" t="n">
         <v>43796</v>
@@ -1443,7 +1446,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>8</v>
@@ -1489,7 +1492,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>16</v>
@@ -1546,7 +1549,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
@@ -1562,10 +1565,10 @@
     </row>
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="12" t="n">
         <v>43771</v>
@@ -1592,10 +1595,10 @@
     </row>
     <row r="32" customFormat="false" ht="41.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="C32" s="12" t="n">
         <v>43778</v>
@@ -1625,10 +1628,10 @@
     </row>
     <row r="33" customFormat="false" ht="40.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C33" s="12" t="n">
         <v>43804</v>
@@ -1659,10 +1662,10 @@
     </row>
     <row r="34" customFormat="false" ht="40.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C34" s="12" t="n">
         <v>43817</v>
@@ -1717,7 +1720,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
@@ -1739,7 +1742,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>8</v>
@@ -1796,7 +1799,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>8</v>
@@ -1855,7 +1858,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>8</v>
@@ -1913,7 +1916,7 @@
     </row>
     <row r="43" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>16</v>
@@ -1944,7 +1947,7 @@
     <row r="44" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10"/>
       <c r="B44" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C44" s="12" t="n">
         <v>43843</v>
@@ -1970,10 +1973,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C45" s="12" t="n">
         <v>43789</v>
@@ -1996,10 +1999,10 @@
       <c r="DD45" s="3"/>
       <c r="DE45" s="0"/>
     </row>
-    <row r="46" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10"/>
       <c r="B46" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C46" s="12" t="n">
         <v>43843</v>
@@ -2019,7 +2022,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
@@ -2035,7 +2038,7 @@
     </row>
     <row r="48" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>8</v>
@@ -2059,7 +2062,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>8</v>
@@ -2081,7 +2084,7 @@
     </row>
     <row r="50" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>8</v>
@@ -2096,7 +2099,7 @@
     </row>
     <row r="51" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>8</v>
@@ -2475,67 +2478,67 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2571,12 +2574,12 @@
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>8</v>
@@ -2622,58 +2625,58 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2681,52 +2684,52 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,27 +2737,27 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>